<commit_message>
Wind can shutdown/startup and FRT modes are control inputs via excel
</commit_message>
<xml_diff>
--- a/resources.xlsx
+++ b/resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\banderso2\Documents\MIRACL\Autonomous-Microgrid-Control-with-Forecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357712A3-CED3-477E-A110-B9B51DE68C6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83387584-694E-4C1A-B8BA-1BAFD462545B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A83621FA-62A6-4AD3-9D39-D6578664D69A}"/>
   </bookViews>
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46F20080-F0BF-4011-A1F5-7DD4F7E0269F}">
-  <dimension ref="A1:B52"/>
+  <dimension ref="A1:B106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B24" sqref="B23:B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B2:B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +500,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -508,7 +508,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -516,7 +516,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -524,7 +524,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -532,7 +532,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -540,7 +540,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -548,7 +548,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -556,7 +556,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -564,7 +564,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -572,7 +572,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -580,7 +580,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -588,7 +588,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -596,7 +596,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -604,7 +604,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -612,7 +612,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -620,7 +620,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -628,7 +628,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -636,7 +636,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -644,7 +644,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -652,7 +652,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -660,7 +660,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -668,7 +668,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -676,7 +676,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -684,7 +684,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -692,7 +692,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -700,7 +700,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -708,7 +708,7 @@
         <v>37</v>
       </c>
       <c r="B39">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -716,7 +716,7 @@
         <v>38</v>
       </c>
       <c r="B40">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -724,7 +724,7 @@
         <v>39</v>
       </c>
       <c r="B41">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -732,7 +732,7 @@
         <v>40</v>
       </c>
       <c r="B42">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -740,7 +740,7 @@
         <v>41</v>
       </c>
       <c r="B43">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -748,7 +748,7 @@
         <v>42</v>
       </c>
       <c r="B44">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -756,7 +756,7 @@
         <v>43</v>
       </c>
       <c r="B45">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -764,7 +764,7 @@
         <v>44</v>
       </c>
       <c r="B46">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -772,7 +772,7 @@
         <v>45</v>
       </c>
       <c r="B47">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -780,7 +780,7 @@
         <v>46</v>
       </c>
       <c r="B48">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -788,22 +788,463 @@
         <v>47</v>
       </c>
       <c r="B49">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
+      <c r="B50">
+        <v>15</v>
+      </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
+      <c r="B51">
+        <v>15</v>
+      </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
+      </c>
+      <c r="B52">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>51</v>
+      </c>
+      <c r="B53">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>52</v>
+      </c>
+      <c r="B54">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>53</v>
+      </c>
+      <c r="B55">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>54</v>
+      </c>
+      <c r="B56">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>55</v>
+      </c>
+      <c r="B57">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>56</v>
+      </c>
+      <c r="B58">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>58</v>
+      </c>
+      <c r="B60">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>59</v>
+      </c>
+      <c r="B61">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>60</v>
+      </c>
+      <c r="B62">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>61</v>
+      </c>
+      <c r="B63">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>62</v>
+      </c>
+      <c r="B64">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>63</v>
+      </c>
+      <c r="B65">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>66</v>
+      </c>
+      <c r="B68">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>68</v>
+      </c>
+      <c r="B70">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>69</v>
+      </c>
+      <c r="B71">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>70</v>
+      </c>
+      <c r="B72">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>71</v>
+      </c>
+      <c r="B73">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <v>72</v>
+      </c>
+      <c r="B74">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <v>75</v>
+      </c>
+      <c r="B77">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <v>76</v>
+      </c>
+      <c r="B78">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <v>77</v>
+      </c>
+      <c r="B79">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <v>78</v>
+      </c>
+      <c r="B80">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82">
+        <v>80</v>
+      </c>
+      <c r="B82">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83">
+        <v>81</v>
+      </c>
+      <c r="B83">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85">
+        <v>83</v>
+      </c>
+      <c r="B85">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86">
+        <v>84</v>
+      </c>
+      <c r="B86">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A87">
+        <v>85</v>
+      </c>
+      <c r="B87">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A88">
+        <v>86</v>
+      </c>
+      <c r="B88">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A89">
+        <v>87</v>
+      </c>
+      <c r="B89">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A90">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A91">
+        <v>89</v>
+      </c>
+      <c r="B91">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A92">
+        <v>90</v>
+      </c>
+      <c r="B92">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A93">
+        <v>91</v>
+      </c>
+      <c r="B93">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A94">
+        <v>92</v>
+      </c>
+      <c r="B94">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A95">
+        <v>93</v>
+      </c>
+      <c r="B95">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A96">
+        <v>94</v>
+      </c>
+      <c r="B96">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A97">
+        <v>95</v>
+      </c>
+      <c r="B97">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A98">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A99">
+        <v>97</v>
+      </c>
+      <c r="B99">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A100">
+        <v>98</v>
+      </c>
+      <c r="B100">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>99</v>
+      </c>
+      <c r="B101">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102">
+        <v>100</v>
+      </c>
+      <c r="B102">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103">
+        <v>101</v>
+      </c>
+      <c r="B103">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104">
+        <v>102</v>
+      </c>
+      <c r="B104">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105">
+        <v>103</v>
+      </c>
+      <c r="B105">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106">
+        <v>104</v>
+      </c>
+      <c r="B106">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Current version 020822. Has islanded mode controller implemented. Still running functionality checks. Diesel switches on at low SOC. PV instability issues patched by keeping in GFM for first 7 sec, then transitioning to GFL. Origin of PV issue unknown.
</commit_message>
<xml_diff>
--- a/resources.xlsx
+++ b/resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\banderso2\Documents\MIRACL\Autonomous-Microgrid-Control-with-Forecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0399A922-A7C1-420E-B18C-5F050AF55330}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4DB08D-7B7E-4583-83A6-0EC39C969466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A83621FA-62A6-4AD3-9D39-D6578664D69A}"/>
   </bookViews>
@@ -393,8 +393,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46F20080-F0BF-4011-A1F5-7DD4F7E0269F}">
   <dimension ref="A1:B106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B15"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +500,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -508,7 +508,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -516,7 +516,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -524,7 +524,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -532,7 +532,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -540,7 +540,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -548,7 +548,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -556,7 +556,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -564,7 +564,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -572,7 +572,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -580,7 +580,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -588,7 +588,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -596,7 +596,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -604,7 +604,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -612,7 +612,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -620,7 +620,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -628,7 +628,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -636,7 +636,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -644,7 +644,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -652,7 +652,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -660,7 +660,7 @@
         <v>31</v>
       </c>
       <c r="B33">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -668,7 +668,7 @@
         <v>32</v>
       </c>
       <c r="B34">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -676,7 +676,7 @@
         <v>33</v>
       </c>
       <c r="B35">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -684,7 +684,7 @@
         <v>34</v>
       </c>
       <c r="B36">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -692,7 +692,7 @@
         <v>35</v>
       </c>
       <c r="B37">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -700,7 +700,7 @@
         <v>36</v>
       </c>
       <c r="B38">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
grid connected and islanded modes working
</commit_message>
<xml_diff>
--- a/resources.xlsx
+++ b/resources.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\banderso2\Documents\MIRACL\Autonomous-Microgrid-Control-with-Forecasting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4DB08D-7B7E-4583-83A6-0EC39C969466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C3E426-2A16-4E57-A3E4-EDE5A227FFC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A83621FA-62A6-4AD3-9D39-D6578664D69A}"/>
   </bookViews>
@@ -394,7 +394,7 @@
   <dimension ref="A1:B106"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+      <selection activeCell="B23" sqref="B23:B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,7 +500,7 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -508,7 +508,7 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -516,7 +516,7 @@
         <v>13</v>
       </c>
       <c r="B15">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -524,7 +524,7 @@
         <v>14</v>
       </c>
       <c r="B16">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -532,7 +532,7 @@
         <v>15</v>
       </c>
       <c r="B17">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -540,7 +540,7 @@
         <v>16</v>
       </c>
       <c r="B18">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -548,7 +548,7 @@
         <v>17</v>
       </c>
       <c r="B19">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -556,7 +556,7 @@
         <v>18</v>
       </c>
       <c r="B20">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -564,7 +564,7 @@
         <v>19</v>
       </c>
       <c r="B21">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -572,7 +572,7 @@
         <v>20</v>
       </c>
       <c r="B22">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -580,7 +580,7 @@
         <v>21</v>
       </c>
       <c r="B23">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -588,7 +588,7 @@
         <v>22</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -596,7 +596,7 @@
         <v>23</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -604,7 +604,7 @@
         <v>24</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -612,7 +612,7 @@
         <v>25</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -620,7 +620,7 @@
         <v>26</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -628,7 +628,7 @@
         <v>27</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -636,7 +636,7 @@
         <v>28</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -644,7 +644,7 @@
         <v>29</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -652,7 +652,7 @@
         <v>30</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>